<commit_message>
Changed log file location to match lab. Changed Template to select correct samAccount name. Moved log entry for groups outside of ForEach loop.
</commit_message>
<xml_diff>
--- a/NewPilotTemplate.xlsx
+++ b/NewPilotTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Scripts\New Pilot AD Accounts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PowerShell\AddNewPilots\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
   <si>
     <t>Last</t>
   </si>
@@ -137,6 +137,42 @@
   </si>
   <si>
     <t>MEM</t>
+  </si>
+  <si>
+    <t>Pilot</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>TUP</t>
+  </si>
+  <si>
+    <t>123 Main St</t>
+  </si>
+  <si>
+    <t>Somewhere, AL 12345</t>
+  </si>
+  <si>
+    <t>555 123 4567</t>
+  </si>
+  <si>
+    <t>123 555 7890</t>
+  </si>
+  <si>
+    <t>example@domain.com</t>
+  </si>
+  <si>
+    <t>1/1/1901</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>SIC</t>
   </si>
 </sst>
 </file>
@@ -146,7 +182,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\&quot;@\&quot;"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,6 +313,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -579,7 +623,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -622,13 +666,15 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -662,6 +708,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -984,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,37 +1109,64 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1" t="e">
+      <c r="A2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" s="1" t="str">
         <f>LEFT(F2,LEN(F2)-10)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O2" s="1" t="e">
+        <v>Somewhere</v>
+      </c>
+      <c r="O2" s="1" t="str">
         <f>MID(F2,(LEN(F2)-8),3)</f>
-        <v>#VALUE!</v>
+        <v xml:space="preserve"> AL</v>
       </c>
       <c r="P2" s="1" t="str">
         <f>RIGHT(F2,5)</f>
-        <v/>
-      </c>
-      <c r="Q2" s="1" t="e">
+        <v>12345</v>
+      </c>
+      <c r="Q2" s="1" t="str">
         <f>VLOOKUP(J2,Sheet1!$A$1:$B$19,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R2" s="2" t="e">
-        <f>IF(M2="PIC",IF(J2="PSM","pc12picpsm",IF(Q2="North","PC12PICRemoteNorth","PC12PICRemoteSouth")),IF(J2="PSM","PC12SICPSM",IF(Q2="North","PC12SICRemoteNorth","PC12SICRemoteSouth")))</f>
-        <v>#N/A</v>
+        <v>South</v>
+      </c>
+      <c r="R2" s="2" t="str">
+        <f>IF(M2="PIC",IF(J2="PSM","pc12picpsm",IF(Q2="North","PC12PICRemoteN","PC12PICRemoteS")),IF(J2="PSM","PC12SICPSM",IF(Q2="North","PC12SICRemoteN","PC12SICRemoteS")))</f>
+        <v>PC12SICRemoteS</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -1108,26 +1182,11 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="1" t="e">
-        <f t="shared" ref="N3:N11" si="0">LEFT(F3,LEN(F3)-10)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O3" s="1" t="e">
-        <f t="shared" ref="O3:O11" si="1">MID(F3,(LEN(F3)-8),3)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P3" s="1" t="str">
-        <f t="shared" ref="P3:P11" si="2">RIGHT(F3,5)</f>
-        <v/>
-      </c>
-      <c r="Q3" s="1" t="e">
-        <f>VLOOKUP(J3,Sheet1!$A$1:$B$19,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R3" s="2" t="e">
-        <f t="shared" ref="R3:R11" si="3">IF(M3="PIC",IF(J3="PSM","pc12picpsm",IF(Q3="North","PC12PICRemoteNorth","PC12PICRemoteSouth")),IF(J3="PSM","PC12SICPSM",IF(Q3="North","PC12SICRemoteNorth","PC12SICRemoteSouth")))</f>
-        <v>#N/A</v>
-      </c>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="2"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -1142,26 +1201,11 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O4" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P4" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="Q4" s="1" t="e">
-        <f>VLOOKUP(J4,Sheet1!$A$1:$B$19,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R4" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -1176,26 +1220,11 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O5" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P5" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="Q5" s="1" t="e">
-        <f>VLOOKUP(J5,Sheet1!$A$1:$B$19,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R5" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -1210,26 +1239,11 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O6" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P6" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="Q6" s="1" t="e">
-        <f>VLOOKUP(J6,Sheet1!$A$1:$B$19,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R6" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -1244,26 +1258,11 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O7" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P7" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="Q7" s="1" t="e">
-        <f>VLOOKUP(J7,Sheet1!$A$1:$B$19,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R7" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -1278,26 +1277,11 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O8" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P8" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="Q8" s="1" t="e">
-        <f>VLOOKUP(J8,Sheet1!$A$1:$B$19,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R8" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
@@ -1312,26 +1296,11 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O9" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P9" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="Q9" s="1" t="e">
-        <f>VLOOKUP(J9,Sheet1!$A$1:$B$19,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R9" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -1346,26 +1315,11 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O10" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P10" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="Q10" s="1" t="e">
-        <f>VLOOKUP(J10,Sheet1!$A$1:$B$19,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R10" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -1380,30 +1334,18 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O11" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P11" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="Q11" s="1" t="e">
-        <f>VLOOKUP(J11,Sheet1!$A$1:$B$19,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R11" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Corrected lab AD. Reverted Template field change in NewPilotTemplate.
</commit_message>
<xml_diff>
--- a/NewPilotTemplate.xlsx
+++ b/NewPilotTemplate.xlsx
@@ -1031,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:R11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,8 +1165,8 @@
         <v>South</v>
       </c>
       <c r="R2" s="2" t="str">
-        <f>IF(M2="PIC",IF(J2="PSM","pc12picpsm",IF(Q2="North","PC12PICRemoteN","PC12PICRemoteS")),IF(J2="PSM","PC12SICPSM",IF(Q2="North","PC12SICRemoteN","PC12SICRemoteS")))</f>
-        <v>PC12SICRemoteS</v>
+        <f>IF(M2="PIC",IF(J2="PSM","pc12picpsm",IF(Q2="North","PC12PICRemoteNorth","PC12PICRemoteSouth")),IF(J2="PSM","PC12SICPSM",IF(Q2="North","PC12SICRemoteNorth","PC12SICRemoteSouth")))</f>
+        <v>PC12SICRemoteSouth</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>